<commit_message>
Finally got adapter extension override to work
</commit_message>
<xml_diff>
--- a/WorkBot/refactor/data/orders/A.L. George/A.L. George_Triphammer_2025-08-07.xlsx
+++ b/WorkBot/refactor/data/orders/A.L. George/A.L. George_Triphammer_2025-08-07.xlsx
@@ -515,7 +515,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -525,7 +525,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>28.75</t>
+          <t>57.50</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -552,7 +552,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>28.75</t>
+          <t>57.50</t>
         </is>
       </c>
     </row>

</xml_diff>